<commit_message>
mise ajour Asserve definitif
</commit_message>
<xml_diff>
--- a/Module Moteur/Software/ReadArduinoSerial/out/production/ReadArduinoSerial/ReponsePIDMethodeCalculatoire.xlsx
+++ b/Module Moteur/Software/ReadArduinoSerial/out/production/ReadArduinoSerial/ReponsePIDMethodeCalculatoire.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21943" windowHeight="8126" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21943" windowHeight="8126"/>
   </bookViews>
   <sheets>
     <sheet name="r0 = 19.786 r1 = -2.817 " sheetId="1" r:id="rId1"/>
@@ -19,6 +19,14 @@
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>e</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13451,14 +13459,14 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>666749</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>46264</xdr:rowOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>21771</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>397328</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>13607</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>348343</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>174171</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -13783,9 +13791,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D999"/>
+  <dimension ref="B1:E999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -13967,7 +13975,7 @@
         <v>0.21023</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B17">
         <v>5322</v>
       </c>
@@ -13978,7 +13986,7 @@
         <v>0.236508</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B18">
         <v>5342</v>
       </c>
@@ -13989,7 +13997,7 @@
         <v>0.26607199999999998</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B19">
         <v>5362</v>
       </c>
@@ -13999,8 +14007,11 @@
       <c r="D19">
         <v>0.29563600000000001</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="E19" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B20">
         <v>5382</v>
       </c>
@@ -14011,7 +14022,7 @@
         <v>0.33176899999999998</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B21">
         <v>5402</v>
       </c>
@@ -14022,7 +14033,7 @@
         <v>0.35804799999999998</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B22">
         <v>5422</v>
       </c>
@@ -14033,7 +14044,7 @@
         <v>0.38432699999999997</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B23">
         <v>5442</v>
       </c>
@@ -14044,7 +14055,7 @@
         <v>0.40732000000000002</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B24">
         <v>5462</v>
       </c>
@@ -14055,7 +14066,7 @@
         <v>0.43031399999999997</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B25">
         <v>5482</v>
       </c>
@@ -14066,7 +14077,7 @@
         <v>0.45002300000000001</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B26">
         <v>5502</v>
       </c>
@@ -14077,7 +14088,7 @@
         <v>0.46973300000000001</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B27">
         <v>5522</v>
       </c>
@@ -14088,7 +14099,7 @@
         <v>0.49929600000000002</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B28">
         <v>5542</v>
       </c>
@@ -14099,7 +14110,7 @@
         <v>0.512436</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B29">
         <v>5562</v>
       </c>
@@ -14110,7 +14121,7 @@
         <v>0.54528399999999999</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B30">
         <v>5582</v>
       </c>
@@ -14121,7 +14132,7 @@
         <v>0.53871400000000003</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B31">
         <v>5602</v>
       </c>
@@ -14132,7 +14143,7 @@
         <v>0.56170799999999999</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B32">
         <v>5622</v>
       </c>
@@ -45706,7 +45717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A14:C913"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A229" workbookViewId="0">
+    <sheetView topLeftCell="A229" workbookViewId="0">
       <selection activeCell="J244" sqref="J244"/>
     </sheetView>
   </sheetViews>

</xml_diff>